<commit_message>
FUNCTIONALITY: SourceProviderRDO - Wrote a new test case.
</commit_message>
<xml_diff>
--- a/QA/Tests/RDOs/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/RDOs/_Test_Suite_Statistics.xlsx
@@ -538,7 +538,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,10 +611,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>7</v>
@@ -628,7 +628,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C$2:C36)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B$2:B36)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FUNCTIONALITY: Updated the RDO Test Suites.
</commit_message>
<xml_diff>
--- a/QA/Tests/RDOs/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/RDOs/_Test_Suite_Statistics.xlsx
@@ -538,7 +538,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,10 +590,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
@@ -628,7 +628,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C$2:C36)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B$2:B36)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FUNCTIONALITY: Updated the test suites.
</commit_message>
<xml_diff>
--- a/QA/Tests/RDOs/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/RDOs/_Test_Suite_Statistics.xlsx
@@ -538,7 +538,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,10 +611,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>7</v>
@@ -628,7 +628,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C$2:C36)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B$2:B36)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FUNCTIONALITY: Wrote new suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/RDOs/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/RDOs/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Title</t>
   </si>
@@ -150,7 +150,141 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -538,7 +672,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +702,7 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) -1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -582,18 +716,18 @@
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
@@ -603,18 +737,18 @@
       </c>
       <c r="G2" s="7">
         <f>COUNTIF($D:$D,"Automated")+COUNTIF($D:$D,"Finished")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>7</v>
@@ -623,12 +757,24 @@
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -637,7 +783,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -664,34 +810,60 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D1 D4:D1048576">
-    <cfRule type="containsText" dxfId="8" priority="14" operator="containsText" text="Outdated">
+  <conditionalFormatting sqref="D5:D1048576 D1">
+    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="Outdated">
       <formula>NOT(ISERROR(SEARCH("Outdated",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D3">
-    <cfRule type="containsText" dxfId="7" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+  <conditionalFormatting sqref="D3:D4">
+    <cfRule type="containsText" dxfId="23" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="16" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+      <formula>NOT(ISERROR(SEARCH("Suited to Manual",D3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="containsText" dxfId="15" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="14" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="13" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="12" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="11" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="10" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="9" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+    <cfRule type="containsText" dxfId="8" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
       <formula>NOT(ISERROR(SEARCH("Suited to Manual",D2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>